<commit_message>
API: Gameweeks import (#25)
</commit_message>
<xml_diff>
--- a/api/tests/imports/challenge/challenge_import_choice_element_not_object.xlsx
+++ b/api/tests/imports/challenge/challenge_import_choice_element_not_object.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -72,6 +72,12 @@
     <t>Skill LongTermVision</t>
   </si>
   <si>
+    <t>Show Statistics Continuously</t>
+  </si>
+  <si>
+    <t>Gameweek</t>
+  </si>
+  <si>
     <t>C001</t>
   </si>
   <si>
@@ -88,6 +94,9 @@
   </si>
   <si>
     <t>2024-12-31 23:59:59</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
   <si>
     <t>Challenge ID</t>
@@ -460,7 +469,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +477,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,28 +532,34 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F2">
         <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K2">
         <v>10</v>
@@ -569,6 +584,12 @@
       </c>
       <c r="R2">
         <v>10</v>
+      </c>
+      <c r="S2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -593,45 +614,45 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H2">
         <v>1</v>

</xml_diff>